<commit_message>
Cuadro resumen + Área de control
Creación de cuadro resumen con su debida explicación. Creación de área de control con el análisis de los gráficos.
</commit_message>
<xml_diff>
--- a/Instrumento TEG/Boxsteps - Instrumento (Respuestas).xlsx
+++ b/Instrumento TEG/Boxsteps - Instrumento (Respuestas).xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resultados" sheetId="1" r:id="rId1"/>
-    <sheet name="Preguntas" sheetId="3" r:id="rId2"/>
-    <sheet name="Preguntas agrupadas" sheetId="6" r:id="rId3"/>
+    <sheet name="Aserciones" sheetId="3" r:id="rId2"/>
+    <sheet name="Aserciones agrupadas" sheetId="6" r:id="rId3"/>
     <sheet name="Análisis" sheetId="2" r:id="rId4"/>
     <sheet name="Gráficos planificación" sheetId="4" r:id="rId5"/>
     <sheet name="Gráficos control y supervisión" sheetId="5" r:id="rId6"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="158">
   <si>
     <t>Timestamp</t>
   </si>
@@ -224,111 +224,6 @@
     <t>Educación Integral</t>
   </si>
   <si>
-    <t>P10</t>
-  </si>
-  <si>
-    <t>P11</t>
-  </si>
-  <si>
-    <t>P12</t>
-  </si>
-  <si>
-    <t>P13</t>
-  </si>
-  <si>
-    <t>P14</t>
-  </si>
-  <si>
-    <t>P15</t>
-  </si>
-  <si>
-    <t>P16</t>
-  </si>
-  <si>
-    <t>P17</t>
-  </si>
-  <si>
-    <t>P18</t>
-  </si>
-  <si>
-    <t>P19</t>
-  </si>
-  <si>
-    <t>P20</t>
-  </si>
-  <si>
-    <t>P21</t>
-  </si>
-  <si>
-    <t>P22</t>
-  </si>
-  <si>
-    <t>P23</t>
-  </si>
-  <si>
-    <t>P24</t>
-  </si>
-  <si>
-    <t>P25</t>
-  </si>
-  <si>
-    <t>P26</t>
-  </si>
-  <si>
-    <t>P27</t>
-  </si>
-  <si>
-    <t>P28</t>
-  </si>
-  <si>
-    <t>P29</t>
-  </si>
-  <si>
-    <t>P30</t>
-  </si>
-  <si>
-    <t>P31</t>
-  </si>
-  <si>
-    <t>P32</t>
-  </si>
-  <si>
-    <t>P33</t>
-  </si>
-  <si>
-    <t>P34</t>
-  </si>
-  <si>
-    <t>P35</t>
-  </si>
-  <si>
-    <t>P01</t>
-  </si>
-  <si>
-    <t>P02</t>
-  </si>
-  <si>
-    <t>P03</t>
-  </si>
-  <si>
-    <t>P04</t>
-  </si>
-  <si>
-    <t>P05</t>
-  </si>
-  <si>
-    <t>P06</t>
-  </si>
-  <si>
-    <t>P07</t>
-  </si>
-  <si>
-    <t>P08</t>
-  </si>
-  <si>
-    <t>P09</t>
-  </si>
-  <si>
     <t>C01</t>
   </si>
   <si>
@@ -392,7 +287,217 @@
     <t>CG - Conocimiento general</t>
   </si>
   <si>
-    <t>Preguntas</t>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>29</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>33</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+  <si>
+    <t>35</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>A04</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>A06</t>
+  </si>
+  <si>
+    <t>A07</t>
+  </si>
+  <si>
+    <t>A08</t>
+  </si>
+  <si>
+    <t>A09</t>
+  </si>
+  <si>
+    <t>A10</t>
+  </si>
+  <si>
+    <t>A11</t>
+  </si>
+  <si>
+    <t>A12</t>
+  </si>
+  <si>
+    <t>A13</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>A16</t>
+  </si>
+  <si>
+    <t>A17</t>
+  </si>
+  <si>
+    <t>A18</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>A20</t>
+  </si>
+  <si>
+    <t>A21</t>
+  </si>
+  <si>
+    <t>A22</t>
+  </si>
+  <si>
+    <t>A23</t>
+  </si>
+  <si>
+    <t>A24</t>
+  </si>
+  <si>
+    <t>A25</t>
+  </si>
+  <si>
+    <t>A26</t>
+  </si>
+  <si>
+    <t>A27</t>
+  </si>
+  <si>
+    <t>A28</t>
+  </si>
+  <si>
+    <t>A29</t>
+  </si>
+  <si>
+    <t>A30</t>
+  </si>
+  <si>
+    <t>A31</t>
+  </si>
+  <si>
+    <t>A32</t>
+  </si>
+  <si>
+    <t>A33</t>
+  </si>
+  <si>
+    <t>A34</t>
+  </si>
+  <si>
+    <t>A35</t>
+  </si>
+  <si>
+    <t>Aserciones</t>
   </si>
 </sst>
 </file>
@@ -457,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -472,6 +577,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -893,7 +1005,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$2</c:f>
+              <c:f>Aserciones!$F$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1344,7 +1456,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$11</c:f>
+              <c:f>Aserciones!$F$11</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1755,6 +1867,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1794,7 +1907,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$12</c:f>
+              <c:f>Aserciones!$F$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2044,7 +2157,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2121,6 +2236,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2202,6 +2318,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2241,7 +2358,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$13</c:f>
+              <c:f>Aserciones!$F$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2491,7 +2608,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -2568,6 +2687,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2649,6 +2769,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2688,7 +2809,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$14</c:f>
+              <c:f>Aserciones!$F$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2938,7 +3059,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -3015,6 +3138,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3136,7 +3260,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$15</c:f>
+              <c:f>Aserciones!$F$15</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3587,7 +3711,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$16</c:f>
+              <c:f>Aserciones!$F$16</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3998,6 +4122,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4037,7 +4162,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$17</c:f>
+              <c:f>Aserciones!$F$17</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4287,7 +4412,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -4364,6 +4491,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4445,6 +4573,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4484,7 +4613,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$18</c:f>
+              <c:f>Aserciones!$F$18</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4734,7 +4863,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -4811,6 +4942,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4892,6 +5024,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4931,7 +5064,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$19</c:f>
+              <c:f>Aserciones!$F$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5181,7 +5314,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -5258,6 +5393,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5339,6 +5475,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5378,7 +5515,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$20</c:f>
+              <c:f>Aserciones!$F$20</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -5628,7 +5765,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -5705,6 +5844,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5826,7 +5966,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$3</c:f>
+              <c:f>Aserciones!$F$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6237,6 +6377,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6276,7 +6417,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$21</c:f>
+              <c:f>Aserciones!$F$21</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -6526,7 +6667,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -6603,6 +6746,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -6724,7 +6868,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$22</c:f>
+              <c:f>Aserciones!$F$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7175,7 +7319,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$23</c:f>
+              <c:f>Aserciones!$F$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7586,6 +7730,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -7625,7 +7770,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$24</c:f>
+              <c:f>Aserciones!$F$24</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -7875,7 +8020,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -7952,6 +8099,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8033,6 +8181,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8072,7 +8221,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$25</c:f>
+              <c:f>Aserciones!$F$25</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8322,7 +8471,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -8399,6 +8550,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8480,6 +8632,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8519,7 +8672,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$26</c:f>
+              <c:f>Aserciones!$F$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -8769,7 +8922,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -8846,6 +9001,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8927,6 +9083,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8966,7 +9123,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$27</c:f>
+              <c:f>Aserciones!$F$27</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9216,7 +9373,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -9293,6 +9452,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9374,6 +9534,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9413,7 +9574,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$28</c:f>
+              <c:f>Aserciones!$F$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -9663,7 +9824,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -9740,6 +9903,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9821,6 +9985,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9860,7 +10025,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$29</c:f>
+              <c:f>Aserciones!$F$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -10110,7 +10275,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -10187,6 +10354,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10268,6 +10436,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10307,7 +10476,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$30</c:f>
+              <c:f>Aserciones!$F$30</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -10557,7 +10726,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -10634,6 +10805,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10755,7 +10927,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$4</c:f>
+              <c:f>Aserciones!$F$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11166,6 +11338,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11205,7 +11378,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$31</c:f>
+              <c:f>Aserciones!$F$31</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11455,7 +11628,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -11532,6 +11707,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11613,6 +11789,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11652,7 +11829,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$32</c:f>
+              <c:f>Aserciones!$F$32</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -11902,7 +12079,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -11979,6 +12158,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12060,6 +12240,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12099,7 +12280,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$33</c:f>
+              <c:f>Aserciones!$F$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -12349,7 +12530,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -12426,6 +12609,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12507,6 +12691,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12546,7 +12731,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$34</c:f>
+              <c:f>Aserciones!$F$34</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -12796,7 +12981,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -12873,6 +13060,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12954,6 +13142,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12993,7 +13182,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$35</c:f>
+              <c:f>Aserciones!$F$35</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -13243,7 +13432,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -13320,6 +13511,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13401,6 +13593,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13440,7 +13633,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$36</c:f>
+              <c:f>Aserciones!$F$36</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -13690,7 +13883,9 @@
               </c:spPr>
             </c:leaderLines>
             <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:cat>
@@ -13767,6 +13962,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13888,7 +14084,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$5</c:f>
+              <c:f>Aserciones!$F$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -14339,7 +14535,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$6</c:f>
+              <c:f>Aserciones!$F$6</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -14790,7 +14986,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$7</c:f>
+              <c:f>Aserciones!$F$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -15241,7 +15437,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$8</c:f>
+              <c:f>Aserciones!$F$8</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -15692,7 +15888,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$9</c:f>
+              <c:f>Aserciones!$F$9</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -16143,7 +16339,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Preguntas!$F$10</c:f>
+              <c:f>Aserciones!$F$10</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -37081,7 +37277,7 @@
     <filterColumn colId="16" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="17">
-    <tableColumn id="1" name="Preguntas" dataDxfId="16"/>
+    <tableColumn id="1" name="Aserciones" dataDxfId="16"/>
     <tableColumn id="2" name="C01" dataDxfId="15"/>
     <tableColumn id="3" name="C02" dataDxfId="14"/>
     <tableColumn id="4" name="C03" dataDxfId="13"/>
@@ -38766,7 +38962,7 @@
   <dimension ref="B2:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B2" sqref="B2:B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -38776,14 +38972,14 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="8" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -38791,14 +38987,14 @@
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="8" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
@@ -38806,14 +39002,14 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="8" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
@@ -38821,14 +39017,14 @@
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="8" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
@@ -38836,14 +39032,14 @@
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
@@ -38851,14 +39047,14 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="C7">
         <v>2</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -38866,14 +39062,14 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
@@ -38881,14 +39077,14 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>99</v>
+        <v>129</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
@@ -38896,14 +39092,14 @@
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="F10" t="s">
         <v>13</v>
@@ -38911,14 +39107,14 @@
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="8" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
@@ -38926,14 +39122,14 @@
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>67</v>
+        <v>132</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F12" t="s">
         <v>15</v>
@@ -38941,14 +39137,14 @@
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="8" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
@@ -38956,14 +39152,14 @@
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="8" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
@@ -38971,14 +39167,14 @@
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>70</v>
+        <v>135</v>
       </c>
       <c r="C15">
         <v>3</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
@@ -38986,14 +39182,14 @@
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>71</v>
+        <v>136</v>
       </c>
       <c r="C16">
         <v>3</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F16" t="s">
         <v>20</v>
@@ -39001,14 +39197,14 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="C17">
         <v>3</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F17" t="s">
         <v>21</v>
@@ -39016,14 +39212,14 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>73</v>
+        <v>138</v>
       </c>
       <c r="C18">
         <v>3</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F18" t="s">
         <v>22</v>
@@ -39031,14 +39227,14 @@
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>74</v>
+        <v>139</v>
       </c>
       <c r="C19">
         <v>3</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="8" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F19" t="s">
         <v>23</v>
@@ -39046,14 +39242,14 @@
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="C20">
         <v>3</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="8" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="F20" t="s">
         <v>24</v>
@@ -39061,14 +39257,14 @@
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>76</v>
+        <v>141</v>
       </c>
       <c r="C21">
         <v>3</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="8" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="F21" t="s">
         <v>25</v>
@@ -39076,14 +39272,14 @@
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>77</v>
+        <v>142</v>
       </c>
       <c r="C22">
         <v>4</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F22" t="s">
         <v>26</v>
@@ -39091,14 +39287,14 @@
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>78</v>
+        <v>143</v>
       </c>
       <c r="C23">
         <v>4</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="8" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="F23" t="s">
         <v>27</v>
@@ -39106,14 +39302,14 @@
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>79</v>
+        <v>144</v>
       </c>
       <c r="C24">
         <v>4</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F24" t="s">
         <v>28</v>
@@ -39121,14 +39317,14 @@
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>80</v>
+        <v>145</v>
       </c>
       <c r="C25">
         <v>4</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="8" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="F25" t="s">
         <v>29</v>
@@ -39136,14 +39332,14 @@
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>81</v>
+        <v>146</v>
       </c>
       <c r="C26">
         <v>4</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F26" t="s">
         <v>30</v>
@@ -39151,14 +39347,14 @@
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C27">
         <v>4</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="8" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="F27" t="s">
         <v>31</v>
@@ -39166,14 +39362,14 @@
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>83</v>
+        <v>148</v>
       </c>
       <c r="C28">
         <v>4</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="8" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="F28" t="s">
         <v>32</v>
@@ -39181,14 +39377,14 @@
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>84</v>
+        <v>149</v>
       </c>
       <c r="C29">
         <v>4</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="8" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="F29" t="s">
         <v>33</v>
@@ -39196,14 +39392,14 @@
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="C30">
         <v>4</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F30" t="s">
         <v>34</v>
@@ -39211,14 +39407,14 @@
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="C31">
         <v>4</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F31" t="s">
         <v>35</v>
@@ -39226,14 +39422,14 @@
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>87</v>
+        <v>152</v>
       </c>
       <c r="C32">
         <v>4</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F32" t="s">
         <v>36</v>
@@ -39241,14 +39437,14 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>88</v>
+        <v>153</v>
       </c>
       <c r="C33">
         <v>4</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="8" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="F33" t="s">
         <v>37</v>
@@ -39256,14 +39452,14 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="C34">
         <v>4</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="8" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="F34" t="s">
         <v>38</v>
@@ -39271,14 +39467,14 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>90</v>
+        <v>155</v>
       </c>
       <c r="C35">
         <v>4</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="8" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="F35" t="s">
         <v>39</v>
@@ -39286,14 +39482,14 @@
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C36">
         <v>4</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="8" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="F36" t="s">
         <v>40</v>
@@ -39301,27 +39497,27 @@
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -39331,570 +39527,677 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:F42"/>
+  <dimension ref="B2:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="5" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="4" max="5" width="4.7109375" customWidth="1"/>
+    <col min="6" max="6" width="67.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C2">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="14">
         <v>1</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>87</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="8" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
       </c>
+      <c r="G2" s="12">
+        <v>4.4000000000000004</v>
+      </c>
     </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B3" s="14">
         <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>88</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="8" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F3" t="s">
         <v>6</v>
       </c>
+      <c r="G3" s="12">
+        <v>3.5</v>
+      </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B4" s="14">
         <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>89</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="8" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
+      <c r="G4" s="12">
+        <v>3.5</v>
+      </c>
     </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B5" s="14">
         <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>90</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="8" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F5" t="s">
         <v>8</v>
       </c>
+      <c r="G5" s="12">
+        <v>2.5</v>
+      </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C6">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B6" s="14">
         <v>2</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>91</v>
       </c>
       <c r="D6" s="5"/>
       <c r="E6" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F6" t="s">
         <v>9</v>
       </c>
+      <c r="G6" s="12">
+        <v>4.7</v>
+      </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>97</v>
-      </c>
-      <c r="C7">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B7" s="14">
         <v>2</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>92</v>
       </c>
       <c r="D7" s="5"/>
       <c r="E7" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
       </c>
+      <c r="G7" s="12">
+        <v>4.9000000000000004</v>
+      </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>98</v>
-      </c>
-      <c r="C8">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B8" s="14">
         <v>2</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>93</v>
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F8" t="s">
         <v>11</v>
       </c>
+      <c r="G8" s="12">
+        <v>4.7</v>
+      </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>99</v>
-      </c>
-      <c r="C9">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B9" s="14">
         <v>2</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>94</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F9" t="s">
         <v>12</v>
       </c>
+      <c r="G9" s="12">
+        <v>5</v>
+      </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>67</v>
-      </c>
-      <c r="C10">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B10" s="14">
         <v>2</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>97</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F10" t="s">
         <v>15</v>
       </c>
+      <c r="G10" s="12">
+        <v>4.9000000000000004</v>
+      </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="14">
         <v>2</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>96</v>
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="8" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
       </c>
+      <c r="G11" s="12">
+        <v>4.5999999999999996</v>
+      </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
-        <v>100</v>
-      </c>
-      <c r="C12">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="14">
         <v>2</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>95</v>
       </c>
       <c r="D12" s="5"/>
       <c r="E12" s="8" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="F12" t="s">
         <v>13</v>
       </c>
+      <c r="G12" s="12">
+        <v>5</v>
+      </c>
     </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B13" s="14">
         <v>2</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>98</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="8" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="F13" t="s">
         <v>16</v>
       </c>
+      <c r="G13" s="12">
+        <v>2.1</v>
+      </c>
     </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C14">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="14">
         <v>2</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="8" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="F14" t="s">
         <v>17</v>
       </c>
+      <c r="G14" s="12">
+        <v>1.4</v>
+      </c>
     </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>70</v>
-      </c>
-      <c r="C15">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="14">
         <v>3</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>100</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="8" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
       </c>
+      <c r="G15" s="12">
+        <v>4.5999999999999996</v>
+      </c>
     </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C16">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="14">
         <v>3</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>102</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="8" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F16" t="s">
         <v>21</v>
       </c>
+      <c r="G16" s="12">
+        <v>3.9</v>
+      </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C17">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B17" s="14">
         <v>3</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>104</v>
       </c>
       <c r="D17" s="7"/>
       <c r="E17" s="8" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="F17" t="s">
         <v>23</v>
       </c>
+      <c r="G17" s="12">
+        <v>5</v>
+      </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" t="s">
-        <v>75</v>
-      </c>
-      <c r="C18">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="14">
         <v>3</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>105</v>
       </c>
       <c r="D18" s="7"/>
       <c r="E18" s="8" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="F18" t="s">
         <v>24</v>
       </c>
+      <c r="G18" s="12">
+        <v>4.0999999999999996</v>
+      </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C19">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="14">
         <v>3</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>106</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="8" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="F19" t="s">
         <v>25</v>
       </c>
+      <c r="G19" s="12">
+        <v>3.6</v>
+      </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="14">
         <v>3</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>101</v>
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F20" t="s">
         <v>20</v>
       </c>
+      <c r="G20" s="12">
+        <v>4.8</v>
+      </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="14">
         <v>3</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>103</v>
       </c>
       <c r="D21" s="7"/>
       <c r="E21" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F21" t="s">
         <v>22</v>
       </c>
+      <c r="G21" s="12">
+        <v>5</v>
+      </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" t="s">
-        <v>88</v>
-      </c>
-      <c r="C22">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B22" s="14">
         <v>4</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>118</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="8" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="F22" t="s">
         <v>37</v>
       </c>
+      <c r="G22" s="12">
+        <v>4.8</v>
+      </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>89</v>
-      </c>
-      <c r="C23">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="14">
         <v>4</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>119</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="8" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="F23" t="s">
         <v>38</v>
       </c>
+      <c r="G23" s="12">
+        <v>4.9000000000000004</v>
+      </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="14">
         <v>4</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>107</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F24" t="s">
         <v>26</v>
       </c>
+      <c r="G24" s="12">
+        <v>4.8</v>
+      </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" t="s">
-        <v>79</v>
-      </c>
-      <c r="C25">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B25" s="14">
         <v>4</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>109</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F25" t="s">
         <v>28</v>
       </c>
+      <c r="G25" s="12">
+        <v>4.9000000000000004</v>
+      </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" t="s">
-        <v>81</v>
-      </c>
-      <c r="C26">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B26" s="14">
         <v>4</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>111</v>
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F26" t="s">
         <v>30</v>
       </c>
+      <c r="G26" s="12">
+        <v>4.8</v>
+      </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B27" t="s">
-        <v>85</v>
-      </c>
-      <c r="C27">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B27" s="14">
         <v>4</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>115</v>
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F27" t="s">
         <v>34</v>
       </c>
+      <c r="G27" s="12">
+        <v>5</v>
+      </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B28" t="s">
-        <v>86</v>
-      </c>
-      <c r="C28">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B28" s="14">
         <v>4</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>116</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F28" t="s">
         <v>35</v>
       </c>
+      <c r="G28" s="12">
+        <v>4.9000000000000004</v>
+      </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B29" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B29" s="14">
         <v>4</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>117</v>
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="8" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="F29" t="s">
         <v>36</v>
       </c>
+      <c r="G29" s="12">
+        <v>4.9000000000000004</v>
+      </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
-        <v>78</v>
-      </c>
-      <c r="C30">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B30" s="14">
         <v>4</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>108</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="8" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="F30" t="s">
         <v>27</v>
       </c>
+      <c r="G30" s="12">
+        <v>4.5999999999999996</v>
+      </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>90</v>
-      </c>
-      <c r="C31">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B31" s="14">
         <v>4</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>120</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="8" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="F31" t="s">
         <v>39</v>
       </c>
+      <c r="G31" s="12">
+        <v>2.1</v>
+      </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B32" t="s">
-        <v>91</v>
-      </c>
-      <c r="C32">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B32" s="14">
         <v>4</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>121</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="8" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="F32" t="s">
         <v>40</v>
       </c>
+      <c r="G32" s="12">
+        <v>4.8</v>
+      </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>80</v>
-      </c>
-      <c r="C33">
+    <row r="33" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="14">
         <v>4</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>110</v>
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="8" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="F33" t="s">
         <v>29</v>
       </c>
+      <c r="G33" s="12">
+        <v>1.3</v>
+      </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>82</v>
-      </c>
-      <c r="C34">
+    <row r="34" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B34" s="14">
         <v>4</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>112</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="8" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="F34" t="s">
         <v>31</v>
       </c>
+      <c r="G34" s="12">
+        <v>4.8</v>
+      </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>83</v>
-      </c>
-      <c r="C35">
+    <row r="35" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B35" s="14">
         <v>4</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>113</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="8" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="F35" t="s">
         <v>32</v>
       </c>
+      <c r="G35" s="12">
+        <v>4.7</v>
+      </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C36">
+    <row r="36" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B36" s="14">
         <v>4</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>114</v>
       </c>
       <c r="D36" s="6"/>
       <c r="E36" s="8" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="F36" t="s">
         <v>33</v>
       </c>
+      <c r="G36" s="12">
+        <v>4.7</v>
+      </c>
     </row>
-    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
     </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
     </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
     </row>
-    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:F36">
-    <sortCondition ref="C2:C36"/>
+  <sortState ref="B2:G36">
+    <sortCondition ref="B2:B36"/>
     <sortCondition ref="E2:E36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -39905,7 +40208,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -39919,37 +40224,37 @@
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B2" s="10" t="s">
-        <v>122</v>
+        <v>157</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>101</v>
+        <v>66</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>102</v>
+        <v>67</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>103</v>
+        <v>68</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>104</v>
+        <v>69</v>
       </c>
       <c r="G2" s="10" t="s">
-        <v>105</v>
+        <v>70</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>106</v>
+        <v>71</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>107</v>
+        <v>72</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>108</v>
+        <v>73</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
       <c r="L2" s="10" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="M2" s="10" t="s">
         <v>49</v>
@@ -39967,12 +40272,12 @@
         <v>48</v>
       </c>
       <c r="R2" s="10" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B3" s="10" t="s">
-        <v>92</v>
+        <v>122</v>
       </c>
       <c r="C3" s="9">
         <v>3</v>
@@ -40031,7 +40336,7 @@
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B4" s="10" t="s">
-        <v>93</v>
+        <v>123</v>
       </c>
       <c r="C4" s="9">
         <v>2</v>
@@ -40090,7 +40395,7 @@
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" s="10" t="s">
-        <v>94</v>
+        <v>124</v>
       </c>
       <c r="C5" s="9">
         <v>4</v>
@@ -40149,7 +40454,7 @@
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B6" s="10" t="s">
-        <v>95</v>
+        <v>125</v>
       </c>
       <c r="C6" s="9">
         <v>3</v>
@@ -40208,7 +40513,7 @@
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" s="10" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="C7" s="9">
         <v>5</v>
@@ -40267,7 +40572,7 @@
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" s="10" t="s">
-        <v>97</v>
+        <v>127</v>
       </c>
       <c r="C8" s="9">
         <v>5</v>
@@ -40326,7 +40631,7 @@
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9" s="10" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="C9" s="9">
         <v>5</v>
@@ -40385,7 +40690,7 @@
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10" s="10" t="s">
-        <v>99</v>
+        <v>129</v>
       </c>
       <c r="C10" s="9">
         <v>5</v>
@@ -40444,7 +40749,7 @@
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" s="10" t="s">
-        <v>100</v>
+        <v>130</v>
       </c>
       <c r="C11" s="9">
         <v>5</v>
@@ -40503,7 +40808,7 @@
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="C12" s="9">
         <v>4</v>
@@ -40562,7 +40867,7 @@
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13" s="10" t="s">
-        <v>67</v>
+        <v>132</v>
       </c>
       <c r="C13" s="9">
         <v>4</v>
@@ -40621,7 +40926,7 @@
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14" s="10" t="s">
-        <v>68</v>
+        <v>133</v>
       </c>
       <c r="C14" s="9">
         <v>2</v>
@@ -40680,7 +40985,7 @@
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B15" s="10" t="s">
-        <v>69</v>
+        <v>134</v>
       </c>
       <c r="C15" s="9">
         <v>1</v>
@@ -40739,7 +41044,7 @@
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="10" t="s">
-        <v>70</v>
+        <v>135</v>
       </c>
       <c r="C16" s="9">
         <v>5</v>
@@ -40798,7 +41103,7 @@
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" s="10" t="s">
-        <v>71</v>
+        <v>136</v>
       </c>
       <c r="C17" s="9">
         <v>5</v>
@@ -40857,7 +41162,7 @@
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B18" s="10" t="s">
-        <v>72</v>
+        <v>137</v>
       </c>
       <c r="C18" s="9">
         <v>4</v>
@@ -40916,7 +41221,7 @@
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B19" s="10" t="s">
-        <v>73</v>
+        <v>138</v>
       </c>
       <c r="C19" s="9">
         <v>5</v>
@@ -40975,7 +41280,7 @@
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B20" s="10" t="s">
-        <v>74</v>
+        <v>139</v>
       </c>
       <c r="C20" s="9">
         <v>5</v>
@@ -41034,7 +41339,7 @@
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B21" s="10" t="s">
-        <v>75</v>
+        <v>140</v>
       </c>
       <c r="C21" s="9">
         <v>3</v>
@@ -41093,7 +41398,7 @@
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B22" s="10" t="s">
-        <v>76</v>
+        <v>141</v>
       </c>
       <c r="C22" s="9">
         <v>3</v>
@@ -41152,7 +41457,7 @@
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B23" s="10" t="s">
-        <v>77</v>
+        <v>142</v>
       </c>
       <c r="C23" s="9">
         <v>5</v>
@@ -41211,7 +41516,7 @@
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B24" s="10" t="s">
-        <v>78</v>
+        <v>143</v>
       </c>
       <c r="C24" s="9">
         <v>5</v>
@@ -41270,7 +41575,7 @@
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B25" s="10" t="s">
-        <v>79</v>
+        <v>144</v>
       </c>
       <c r="C25" s="9">
         <v>4</v>
@@ -41329,7 +41634,7 @@
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B26" s="10" t="s">
-        <v>80</v>
+        <v>145</v>
       </c>
       <c r="C26" s="9">
         <v>1</v>
@@ -41388,7 +41693,7 @@
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B27" s="10" t="s">
-        <v>81</v>
+        <v>146</v>
       </c>
       <c r="C27" s="9">
         <v>5</v>
@@ -41447,7 +41752,7 @@
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B28" s="10" t="s">
-        <v>82</v>
+        <v>147</v>
       </c>
       <c r="C28" s="9">
         <v>4</v>
@@ -41506,7 +41811,7 @@
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B29" s="10" t="s">
-        <v>83</v>
+        <v>148</v>
       </c>
       <c r="C29" s="9">
         <v>4</v>
@@ -41565,7 +41870,7 @@
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B30" s="10" t="s">
-        <v>84</v>
+        <v>149</v>
       </c>
       <c r="C30" s="9">
         <v>4</v>
@@ -41624,7 +41929,7 @@
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B31" s="10" t="s">
-        <v>85</v>
+        <v>150</v>
       </c>
       <c r="C31" s="9">
         <v>5</v>
@@ -41683,7 +41988,7 @@
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B32" s="10" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="C32" s="9">
         <v>5</v>
@@ -41742,7 +42047,7 @@
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B33" s="10" t="s">
-        <v>87</v>
+        <v>152</v>
       </c>
       <c r="C33" s="9">
         <v>4</v>
@@ -41801,7 +42106,7 @@
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B34" s="10" t="s">
-        <v>88</v>
+        <v>153</v>
       </c>
       <c r="C34" s="9">
         <v>5</v>
@@ -41860,7 +42165,7 @@
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B35" s="10" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="C35" s="9">
         <v>5</v>
@@ -41919,7 +42224,7 @@
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B36" s="10" t="s">
-        <v>90</v>
+        <v>155</v>
       </c>
       <c r="C36" s="9">
         <v>1</v>
@@ -41978,7 +42283,7 @@
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B37" s="10" t="s">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="C37" s="9">
         <v>5</v>
@@ -42046,12 +42351,72 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:J186"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="J25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>3</v>
+      </c>
+      <c r="J48">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>4</v>
+      </c>
+      <c r="J71">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J94">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J117">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J140">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="163" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J163">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="186" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J186">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -42059,12 +42424,111 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A2:J324"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>14</v>
+      </c>
+      <c r="J2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="J25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>16</v>
+      </c>
+      <c r="J48">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>17</v>
+      </c>
+      <c r="J71">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>18</v>
+      </c>
+      <c r="J94">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A117">
+        <v>19</v>
+      </c>
+      <c r="J117">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A140">
+        <v>20</v>
+      </c>
+      <c r="J140">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="163" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J163">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="186" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J186">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="209" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J209">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="232" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J232">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="255" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J255">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="278" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J278">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="301" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J301">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="324" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J324">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Culminación de presentación de resultados
Culminación de la presentación de los resultados englobando todas las áreas necesarias.
</commit_message>
<xml_diff>
--- a/Instrumento TEG/Boxsteps - Instrumento (Respuestas).xlsx
+++ b/Instrumento TEG/Boxsteps - Instrumento (Respuestas).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="Resultados" sheetId="1" r:id="rId1"/>
@@ -37579,7 +37579,7 @@
   </sheetPr>
   <dimension ref="A1:AP11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -38961,9 +38961,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:F42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B36"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -39529,15 +39527,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="6.5703125" customWidth="1"/>
     <col min="4" max="5" width="4.7109375" customWidth="1"/>
-    <col min="6" max="6" width="67.5703125" customWidth="1"/>
+    <col min="6" max="6" width="148.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.2">
@@ -40208,9 +40204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:R37"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -42353,9 +42347,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J186"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -42426,9 +42418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:J324"/>
   <sheetViews>
-    <sheetView topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>